<commit_message>
Fixed some mixer problem
</commit_message>
<xml_diff>
--- a/Documentation/Feedback & ToDoList/4711_GUI_FB_1.3.xlsx
+++ b/Documentation/Feedback & ToDoList/4711_GUI_FB_1.3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="204">
   <si>
     <t>I2C Device Address加上</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -976,6 +976,18 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寄存器表就是L/R-&gt;1/0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>再详细点？？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1106,7 +1118,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1175,6 +1187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="差" xfId="3" builtinId="27"/>
@@ -1215,7 +1228,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1259,7 +1272,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1303,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2037,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2424,7 +2437,7 @@
       </c>
     </row>
     <row r="43" spans="4:8" ht="24" customHeight="1">
-      <c r="E43" s="43">
+      <c r="E43" s="44">
         <v>2</v>
       </c>
       <c r="F43" s="9" t="s">
@@ -2432,7 +2445,7 @@
       </c>
     </row>
     <row r="44" spans="4:8" ht="108">
-      <c r="E44" s="43"/>
+      <c r="E44" s="44"/>
       <c r="F44" s="14" t="s">
         <v>98</v>
       </c>
@@ -2917,6 +2930,9 @@
         <v>186</v>
       </c>
       <c r="G95" s="9"/>
+      <c r="H95" s="43" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="96" spans="4:10" s="40" customFormat="1">
       <c r="E96" s="10">
@@ -2926,6 +2942,9 @@
         <v>187</v>
       </c>
       <c r="G96" s="9"/>
+      <c r="H96" s="43" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="97" spans="4:8" s="40" customFormat="1">
       <c r="E97" s="9"/>
@@ -3061,6 +3080,9 @@
       </c>
       <c r="F112" s="10" t="s">
         <v>188</v>
+      </c>
+      <c r="G112" s="43" t="s">
+        <v>202</v>
       </c>
       <c r="H112" s="10"/>
     </row>
@@ -3085,8 +3107,8 @@
       <c r="G114" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="H114" s="39" t="s">
-        <v>185</v>
+      <c r="H114" s="43" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="115" spans="2:8" s="40" customFormat="1">
@@ -3097,6 +3119,9 @@
       <c r="F115" s="10" t="s">
         <v>189</v>
       </c>
+      <c r="H115" s="43" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="117" spans="2:8">
       <c r="D117" s="19" t="s">
@@ -3165,6 +3190,9 @@
       </c>
       <c r="F123" s="10" t="s">
         <v>190</v>
+      </c>
+      <c r="G123" s="43" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="125" spans="2:8">

</xml_diff>